<commit_message>
Remove: Delete EMD processor configuration and documentation files
- Removed the obsolete `emd_processor_config.yaml` and `emd_processor_documentation.md` files to clean up the resources directory.
- Updated the project structure by eliminating outdated configuration and documentation that are no longer in use.
</commit_message>
<xml_diff>
--- a/resources/Out_format.xlsx
+++ b/resources/Out_format.xlsx
@@ -5,21 +5,18 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gostn\OneDrive\桌面\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\my_github\FlightCheckPy\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E8225988-448B-43A0-9C6F-96E8EFF11EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA63B9C0-03DF-42D9-9209-116068057809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="29040" activeTab="1" xr2:uid="{D6DB75D4-A8CC-4A73-9AF5-6E324AED1BA5}"/>
+    <workbookView xWindow="0" yWindow="2148" windowWidth="16416" windowHeight="12156" activeTab="1" xr2:uid="{D6DB75D4-A8CC-4A73-9AF5-6E324AED1BA5}"/>
   </bookViews>
   <sheets>
     <sheet name="RECEIPT" sheetId="17" r:id="rId1"/>
     <sheet name="SUM" sheetId="11" r:id="rId2"/>
     <sheet name="EMD" sheetId="15" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">EMD!$A$1:$P$32</definedName>
   </definedNames>
@@ -134,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>AIR CHINA MISCELLANEOUS CHARGES ORDER SALES REPORT</t>
   </si>
@@ -211,6 +208,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>支票号</t>
@@ -268,6 +266,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>中国国际航空公司旅费证销售（</t>
@@ -288,6 +287,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>报告</t>
@@ -475,6 +475,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>填开部门名称：</t>
@@ -505,12 +506,12 @@
   <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="182" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="184" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="185" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="186" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="187" formatCode="00000"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="179" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="180" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="181" formatCode="00000"/>
   </numFmts>
   <fonts count="41" x14ac:knownFonts="1">
     <font>
@@ -538,11 +539,13 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -560,6 +563,7 @@
       <b/>
       <sz val="12"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -658,16 +662,19 @@
       <b/>
       <sz val="15"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -688,6 +695,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -718,10 +726,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -1157,32 +1167,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="182" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="184" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="12" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="12" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1245,11 +1255,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="186" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="26" fontId="28" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1280,13 +1290,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="186" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="26" fontId="39" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1312,10 +1322,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1325,7 +1335,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="187" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1375,13 +1385,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="184" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="184" fontId="22" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="185" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1395,9 +1408,6 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1437,13 +1447,13 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="186" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="186" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1452,56 +1462,50 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1515,6 +1519,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1734,35 +1744,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="SUM"/>
-      <sheetName val="MCO"/>
-      <sheetName val="EBT"/>
-      <sheetName val="TKT"/>
-      <sheetName val="TAX"/>
-      <sheetName val="FORMAL RECEIPT"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1">
-        <row r="8">
-          <cell r="M8">
-            <v>5</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2056,7 +2037,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E6"/>
+      <selection activeCell="C8" sqref="C8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2169,10 +2150,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="94"/>
-      <c r="C8" s="95" t="str">
-        <f>IF(G5=0,"NO CASH",SpellNumber(G5))</f>
-        <v>NO CASH</v>
-      </c>
+      <c r="C8" s="95"/>
       <c r="D8" s="95"/>
       <c r="E8" s="95"/>
       <c r="F8" s="95"/>
@@ -2407,7 +2385,7 @@
     <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
@@ -2438,19 +2416,19 @@
       <c r="K2" s="25"/>
     </row>
     <row r="3" spans="1:14" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="106"/>
+      <c r="B3" s="107"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
@@ -2507,32 +2485,32 @@
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="110" t="s">
+      <c r="D7" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="110" t="s">
+      <c r="E7" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="110" t="s">
+      <c r="F7" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="110" t="s">
+      <c r="G7" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="107" t="s">
+      <c r="H7" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="108"/>
-      <c r="J7" s="110" t="s">
+      <c r="I7" s="109"/>
+      <c r="J7" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="110" t="s">
+      <c r="K7" s="104" t="s">
         <v>9</v>
       </c>
       <c r="L7" s="2"/>
@@ -2540,20 +2518,20 @@
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="110"/>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110"/>
-      <c r="F8" s="110"/>
-      <c r="G8" s="110"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="104"/>
       <c r="H8" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
       <c r="L8" s="2"/>
       <c r="M8" s="8"/>
     </row>
@@ -2595,10 +2573,7 @@
         <v>0 EMD</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="15" t="e">
-        <f>[1]MCO!M8</f>
-        <v>#REF!</v>
-      </c>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:14" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
@@ -2615,10 +2590,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="18"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="15">
-        <f>[1]TKT!M8</f>
-        <v>5</v>
-      </c>
+      <c r="M10" s="15"/>
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:14" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2725,9 +2697,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -2797,8 +2767,8 @@
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="C21" s="104"/>
-      <c r="D21" s="105"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="106"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
@@ -2930,18 +2900,18 @@
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
-      <c r="E3" s="147" t="str">
+      <c r="E3" s="145" t="str">
         <f>"报告期间：" &amp; N3 &amp; "至" &amp; N3</f>
         <v>报告期间：1900年1月0日至1900年1月0日</v>
       </c>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="147" t="s">
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="147"/>
+      <c r="K3" s="145"/>
       <c r="L3" s="43"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70" t="str">
@@ -2955,17 +2925,17 @@
       <c r="S3" s="45"/>
     </row>
     <row r="4" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="146" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="148"/>
-      <c r="C4" s="148"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
       <c r="D4" s="74"/>
       <c r="E4" s="74"/>
       <c r="F4" s="75"/>
       <c r="G4" s="76"/>
-      <c r="H4" s="149"/>
-      <c r="I4" s="149"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
       <c r="J4" s="71" t="s">
         <v>76</v>
       </c>
@@ -2992,22 +2962,22 @@
       <c r="D5" s="150" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="148" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="150" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="144" t="s">
+      <c r="G5" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="144" t="s">
+      <c r="H5" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="144" t="s">
+      <c r="I5" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="144" t="s">
+      <c r="J5" s="148" t="s">
         <v>29</v>
       </c>
       <c r="K5" s="150" t="s">
@@ -3026,20 +2996,20 @@
       <c r="P5" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="Q5" s="146"/>
-      <c r="R5" s="146"/>
+      <c r="Q5" s="144"/>
+      <c r="R5" s="144"/>
     </row>
     <row r="6" spans="1:19" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="159"/>
       <c r="B6" s="157"/>
       <c r="C6" s="155"/>
       <c r="D6" s="151"/>
-      <c r="E6" s="145"/>
+      <c r="E6" s="149"/>
       <c r="F6" s="151"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="145"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
       <c r="K6" s="151"/>
       <c r="L6" s="153"/>
       <c r="M6" s="55" t="s">
@@ -3060,12 +3030,12 @@
       <c r="B7" s="157"/>
       <c r="C7" s="155"/>
       <c r="D7" s="151"/>
-      <c r="E7" s="145"/>
+      <c r="E7" s="149"/>
       <c r="F7" s="151"/>
-      <c r="G7" s="145"/>
-      <c r="H7" s="145"/>
-      <c r="I7" s="145"/>
-      <c r="J7" s="145"/>
+      <c r="G7" s="149"/>
+      <c r="H7" s="149"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
       <c r="K7" s="151"/>
       <c r="L7" s="56"/>
       <c r="M7" s="56"/>
@@ -3594,16 +3564,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="H5:H7"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="A4:C4"/>
@@ -3612,6 +3572,14 @@
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="F31:G31"/>
@@ -3622,6 +3590,8 @@
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="K29:P32"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E3:I3"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enhance: Improve Excel file processing and cash total calculation
- Updated the Excel file reading logic to support both XLS and XLSX formats, with appropriate error handling for missing dependencies.
- Refactored cash total calculation to sum values from the 'L' column and convert the total to English for output in the Receipt sheet.
- Enhanced user feedback with informative messages during file processing.
</commit_message>
<xml_diff>
--- a/resources/Out_format.xlsx
+++ b/resources/Out_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\my_github\FlightCheckPy\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA63B9C0-03DF-42D9-9209-116068057809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600116D7-5021-47A6-B36B-A116FA2F5608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2148" windowWidth="16416" windowHeight="12156" activeTab="1" xr2:uid="{D6DB75D4-A8CC-4A73-9AF5-6E324AED1BA5}"/>
+    <workbookView xWindow="0" yWindow="2148" windowWidth="16416" windowHeight="12156" xr2:uid="{D6DB75D4-A8CC-4A73-9AF5-6E324AED1BA5}"/>
   </bookViews>
   <sheets>
     <sheet name="RECEIPT" sheetId="17" r:id="rId1"/>
@@ -38,65 +38,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>OFFICE USE</author>
-  </authors>
-  <commentList>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{11FCD64E-D4A2-4E91-96EF-F00B9B47002B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>KAI:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Can accomendate upto three lines (approximately 10,000)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{82EB5DDE-44DC-4370-944B-B6090BEF09CB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>KAI:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-VBA convert value to English words
-=IF(G5=0,"NO CASH",SpellNumber(G5))</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CA987 CA988 SUP</author>
@@ -1162,7 +1103,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
@@ -1337,59 +1278,47 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="181" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1408,105 +1337,6 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1557,6 +1387,114 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -2032,11 +1970,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40067CD-9956-401A-A618-7A92843119E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40067CD-9956-401A-A618-7A92843119E5}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C8" sqref="C8:I9"/>
     </sheetView>
   </sheetViews>
@@ -2067,11 +2005,11 @@
     <row r="2" spans="1:12" ht="22.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="97" t="s">
+      <c r="D2" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="25"/>
@@ -2080,16 +2018,16 @@
       <c r="A3" s="32"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="99" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
       <c r="J3" s="35"/>
       <c r="K3" s="35"/>
       <c r="L3" s="34"/>
@@ -2112,194 +2050,194 @@
         <v>47</v>
       </c>
       <c r="B5" s="89"/>
-      <c r="C5" s="86">
+      <c r="C5" s="90">
         <f>SUM!C13</f>
         <v>0</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="100" t="s">
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="102">
+      <c r="G5" s="94">
         <f>SUM!G11</f>
         <v>0</v>
       </c>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
       <c r="J6" s="33"/>
       <c r="K6" s="33"/>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="95"/>
-      <c r="I8" s="95"/>
+      <c r="B8" s="156"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="157"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
     </row>
     <row r="9" spans="1:12" ht="49.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
-      <c r="B9" s="94"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
+      <c r="A9" s="156"/>
+      <c r="B9" s="156"/>
+      <c r="C9" s="158"/>
+      <c r="D9" s="158"/>
+      <c r="E9" s="158"/>
+      <c r="F9" s="158"/>
+      <c r="G9" s="158"/>
+      <c r="H9" s="158"/>
+      <c r="I9" s="158"/>
     </row>
     <row r="11" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="89" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="89"/>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
       <c r="F11" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="88">
+      <c r="G11" s="97">
         <f>SUM!C14</f>
         <v>0</v>
       </c>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
       <c r="F12" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="89" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="89"/>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="90"/>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
       <c r="F17" s="31" t="s">
         <v>58</v>
       </c>
       <c r="G17" s="31"/>
-      <c r="H17" s="86" t="s">
+      <c r="H17" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="86"/>
+      <c r="I17" s="90"/>
     </row>
     <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="91" t="s">
+      <c r="B18" s="91"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
+      <c r="G18" s="99"/>
+      <c r="H18" s="91"/>
+      <c r="I18" s="91"/>
     </row>
     <row r="20" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
       <c r="F20" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="88">
+      <c r="G20" s="97">
         <f>SUM!C14</f>
         <v>0</v>
       </c>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="87"/>
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
       <c r="F21" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
     </row>
     <row r="22" spans="1:9" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
@@ -2327,6 +2265,20 @@
     <row r="47" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B20:E21"/>
+    <mergeCell ref="G20:I21"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:I15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="B17:E18"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="C8:I9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="G11:I12"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
@@ -2335,20 +2287,6 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:I6"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="C8:I9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="G11:I12"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="B20:E21"/>
-    <mergeCell ref="G20:I21"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:I15"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B17:E18"/>
-    <mergeCell ref="H17:I18"/>
-    <mergeCell ref="F18:G18"/>
   </mergeCells>
   <phoneticPr fontId="40" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2356,7 +2294,6 @@
   <pageSetup scale="95" fitToHeight="2" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2367,7 +2304,7 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2416,19 +2353,19 @@
       <c r="K2" s="25"/>
     </row>
     <row r="3" spans="1:14" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="103" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
@@ -2485,32 +2422,32 @@
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="104" t="s">
+      <c r="F7" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="104" t="s">
+      <c r="G7" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="108" t="s">
+      <c r="H7" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="109"/>
-      <c r="J7" s="104" t="s">
+      <c r="I7" s="105"/>
+      <c r="J7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="104" t="s">
+      <c r="K7" s="100" t="s">
         <v>9</v>
       </c>
       <c r="L7" s="2"/>
@@ -2518,20 +2455,20 @@
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
+      <c r="B8" s="106"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
       <c r="H8" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="104"/>
-      <c r="K8" s="104"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
       <c r="L8" s="2"/>
       <c r="M8" s="8"/>
     </row>
@@ -2767,8 +2704,8 @@
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="C21" s="105"/>
-      <c r="D21" s="106"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="102"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
@@ -2849,47 +2786,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
       <c r="Q1" s="72"/>
       <c r="R1" s="72"/>
       <c r="S1" s="72"/>
     </row>
     <row r="2" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="P2" s="124"/>
       <c r="Q2" s="73"/>
       <c r="R2" s="73"/>
       <c r="S2" s="73"/>
@@ -2900,18 +2837,18 @@
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
-      <c r="E3" s="145" t="str">
+      <c r="E3" s="108" t="str">
         <f>"报告期间：" &amp; N3 &amp; "至" &amp; N3</f>
         <v>报告期间：1900年1月0日至1900年1月0日</v>
       </c>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
-      <c r="J3" s="145" t="s">
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="145"/>
+      <c r="K3" s="108"/>
       <c r="L3" s="43"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70" t="str">
@@ -2925,17 +2862,17 @@
       <c r="S3" s="45"/>
     </row>
     <row r="4" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="146" t="s">
+      <c r="A4" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="146"/>
-      <c r="C4" s="146"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
       <c r="D4" s="74"/>
       <c r="E4" s="74"/>
       <c r="F4" s="75"/>
       <c r="G4" s="76"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
       <c r="J4" s="71" t="s">
         <v>76</v>
       </c>
@@ -2950,68 +2887,68 @@
       <c r="P4" s="71"/>
     </row>
     <row r="5" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="158" t="s">
+      <c r="A5" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="156" t="s">
+      <c r="B5" s="119" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="154" t="s">
+      <c r="C5" s="117" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="150" t="s">
+      <c r="D5" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="150" t="s">
+      <c r="F5" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="148" t="s">
+      <c r="G5" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="148" t="s">
+      <c r="H5" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="148" t="s">
+      <c r="I5" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="148" t="s">
+      <c r="J5" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="150" t="s">
+      <c r="K5" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="152" t="s">
+      <c r="L5" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="152" t="s">
+      <c r="M5" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="N5" s="152"/>
+      <c r="N5" s="115"/>
       <c r="O5" s="59" t="s">
         <v>66</v>
       </c>
       <c r="P5" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="Q5" s="144"/>
-      <c r="R5" s="144"/>
+      <c r="Q5" s="107"/>
+      <c r="R5" s="107"/>
     </row>
     <row r="6" spans="1:19" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="159"/>
-      <c r="B6" s="157"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="151"/>
-      <c r="E6" s="149"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="149"/>
-      <c r="H6" s="149"/>
-      <c r="I6" s="149"/>
-      <c r="J6" s="149"/>
-      <c r="K6" s="151"/>
-      <c r="L6" s="153"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="112"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="116"/>
       <c r="M6" s="55" t="s">
         <v>43</v>
       </c>
@@ -3026,17 +2963,17 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="159"/>
-      <c r="B7" s="157"/>
-      <c r="C7" s="155"/>
-      <c r="D7" s="151"/>
-      <c r="E7" s="149"/>
-      <c r="F7" s="151"/>
-      <c r="G7" s="149"/>
-      <c r="H7" s="149"/>
-      <c r="I7" s="149"/>
-      <c r="J7" s="149"/>
-      <c r="K7" s="151"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="114"/>
       <c r="L7" s="56"/>
       <c r="M7" s="56"/>
       <c r="N7" s="56"/>
@@ -3448,31 +3385,31 @@
       <c r="A29" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="129">
+      <c r="B29" s="141">
         <f>B30+F30</f>
         <v>0</v>
       </c>
-      <c r="C29" s="130"/>
-      <c r="D29" s="131"/>
+      <c r="C29" s="142"/>
+      <c r="D29" s="143"/>
       <c r="E29" s="47" t="s">
         <v>30</v>
       </c>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
-      <c r="H29" s="115" t="s">
+      <c r="H29" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="116"/>
-      <c r="J29" s="117"/>
-      <c r="K29" s="135">
+      <c r="I29" s="128"/>
+      <c r="J29" s="129"/>
+      <c r="K29" s="147">
         <f>B31</f>
         <v>0</v>
       </c>
-      <c r="L29" s="136"/>
-      <c r="M29" s="136"/>
-      <c r="N29" s="136"/>
-      <c r="O29" s="136"/>
-      <c r="P29" s="137"/>
+      <c r="L29" s="148"/>
+      <c r="M29" s="148"/>
+      <c r="N29" s="148"/>
+      <c r="O29" s="148"/>
+      <c r="P29" s="149"/>
       <c r="Q29" s="48"/>
       <c r="R29" s="49"/>
     </row>
@@ -3480,29 +3417,29 @@
       <c r="A30" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="132">
+      <c r="B30" s="144">
         <f>L28</f>
         <v>0</v>
       </c>
-      <c r="C30" s="133"/>
-      <c r="D30" s="134"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="146"/>
       <c r="E30" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="132">
+      <c r="F30" s="144">
         <f>M28+N28</f>
         <v>0</v>
       </c>
-      <c r="G30" s="134"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="119"/>
-      <c r="J30" s="120"/>
-      <c r="K30" s="138"/>
-      <c r="L30" s="139"/>
-      <c r="M30" s="139"/>
-      <c r="N30" s="139"/>
-      <c r="O30" s="139"/>
-      <c r="P30" s="140"/>
+      <c r="G30" s="146"/>
+      <c r="H30" s="130"/>
+      <c r="I30" s="131"/>
+      <c r="J30" s="132"/>
+      <c r="K30" s="150"/>
+      <c r="L30" s="151"/>
+      <c r="M30" s="151"/>
+      <c r="N30" s="151"/>
+      <c r="O30" s="151"/>
+      <c r="P30" s="152"/>
       <c r="Q30" s="48"/>
       <c r="R30" s="49"/>
     </row>
@@ -3510,29 +3447,29 @@
       <c r="A31" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="124">
+      <c r="B31" s="136">
         <f>K28</f>
         <v>0</v>
       </c>
-      <c r="C31" s="125"/>
-      <c r="D31" s="126"/>
+      <c r="C31" s="137"/>
+      <c r="D31" s="138"/>
       <c r="E31" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="113">
+      <c r="F31" s="125">
         <f>D28</f>
         <v>0</v>
       </c>
-      <c r="G31" s="114"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="119"/>
-      <c r="J31" s="120"/>
-      <c r="K31" s="138"/>
-      <c r="L31" s="139"/>
-      <c r="M31" s="139"/>
-      <c r="N31" s="139"/>
-      <c r="O31" s="139"/>
-      <c r="P31" s="140"/>
+      <c r="G31" s="126"/>
+      <c r="H31" s="130"/>
+      <c r="I31" s="131"/>
+      <c r="J31" s="132"/>
+      <c r="K31" s="150"/>
+      <c r="L31" s="151"/>
+      <c r="M31" s="151"/>
+      <c r="N31" s="151"/>
+      <c r="O31" s="151"/>
+      <c r="P31" s="152"/>
       <c r="Q31" s="48"/>
       <c r="R31" s="49"/>
     </row>
@@ -3541,29 +3478,41 @@
         <v>38</v>
       </c>
       <c r="B32" s="68"/>
-      <c r="C32" s="127">
+      <c r="C32" s="139">
         <v>0</v>
       </c>
-      <c r="D32" s="128"/>
+      <c r="D32" s="140"/>
       <c r="E32" s="68" t="s">
         <v>39</v>
       </c>
       <c r="F32" s="68"/>
       <c r="G32" s="68"/>
-      <c r="H32" s="121"/>
-      <c r="I32" s="122"/>
-      <c r="J32" s="123"/>
-      <c r="K32" s="141"/>
-      <c r="L32" s="142"/>
-      <c r="M32" s="142"/>
-      <c r="N32" s="142"/>
-      <c r="O32" s="142"/>
-      <c r="P32" s="143"/>
+      <c r="H32" s="133"/>
+      <c r="I32" s="134"/>
+      <c r="J32" s="135"/>
+      <c r="K32" s="153"/>
+      <c r="L32" s="154"/>
+      <c r="M32" s="154"/>
+      <c r="N32" s="154"/>
+      <c r="O32" s="154"/>
+      <c r="P32" s="155"/>
       <c r="Q32" s="49"/>
       <c r="R32" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H29:J32"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K29:P32"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E3:I3"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="A4:C4"/>
@@ -3580,18 +3529,6 @@
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="J5:J7"/>
     <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H29:J32"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="K29:P32"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E3:I3"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enhance: Improve Excel file column validation and mapping logic
- Updated the column validation to support both English and Chinese column names, ensuring essential columns are checked accurately.
- Introduced a new function to convert numeric values to strings without decimals for better data handling.
- Refactored the output row creation logic to align with the correct mapping based on user requirements, enhancing data integrity in the output file.
</commit_message>
<xml_diff>
--- a/resources/Out_format.xlsx
+++ b/resources/Out_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\my_github\FlightCheckPy\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600116D7-5021-47A6-B36B-A116FA2F5608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C720C9-23EE-41E0-8162-CE60DC3D8BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2148" windowWidth="16416" windowHeight="12156" xr2:uid="{D6DB75D4-A8CC-4A73-9AF5-6E324AED1BA5}"/>
+    <workbookView xWindow="9084" yWindow="3456" windowWidth="16416" windowHeight="12156" xr2:uid="{D6DB75D4-A8CC-4A73-9AF5-6E324AED1BA5}"/>
   </bookViews>
   <sheets>
     <sheet name="RECEIPT" sheetId="17" r:id="rId1"/>
@@ -1278,6 +1278,30 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="181" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed"/>
     </xf>
@@ -1287,15 +1311,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1307,18 +1322,6 @@
     </xf>
     <xf numFmtId="178" fontId="22" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1337,13 +1340,118 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="26" fontId="3" fillId="0" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1354,12 +1462,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1388,113 +1490,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -2005,11 +2005,11 @@
     <row r="2" spans="1:12" ht="22.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="25"/>
@@ -2018,16 +2018,16 @@
       <c r="A3" s="32"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="88" t="s">
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
       <c r="J3" s="35"/>
       <c r="K3" s="35"/>
       <c r="L3" s="34"/>
@@ -2050,44 +2050,44 @@
         <v>47</v>
       </c>
       <c r="B5" s="89"/>
-      <c r="C5" s="90">
+      <c r="C5" s="86">
         <f>SUM!C13</f>
         <v>0</v>
       </c>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="92" t="s">
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="94">
+      <c r="G5" s="99">
         <f>SUM!G11</f>
         <v>0</v>
       </c>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="96"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
       <c r="J6" s="33"/>
       <c r="K6" s="33"/>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="156" t="s">
+      <c r="A8" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="156"/>
+      <c r="B8" s="93"/>
       <c r="C8" s="157"/>
       <c r="D8" s="157"/>
       <c r="E8" s="157"/>
@@ -2097,8 +2097,8 @@
       <c r="I8" s="157"/>
     </row>
     <row r="9" spans="1:12" ht="49.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="156"/>
-      <c r="B9" s="156"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="93"/>
       <c r="C9" s="158"/>
       <c r="D9" s="158"/>
       <c r="E9" s="158"/>
@@ -2112,132 +2112,132 @@
         <v>19</v>
       </c>
       <c r="B11" s="89"/>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
       <c r="F11" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G11" s="88">
         <f>SUM!C14</f>
         <v>0</v>
       </c>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="96" t="s">
+      <c r="A12" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="96"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="91"/>
-      <c r="H12" s="91"/>
-      <c r="I12" s="91"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="89" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="89"/>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="96" t="s">
+      <c r="A15" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="96"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="91"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="90" t="s">
+      <c r="B17" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
       <c r="F17" s="31" t="s">
         <v>58</v>
       </c>
       <c r="G17" s="31"/>
-      <c r="H17" s="90" t="s">
+      <c r="H17" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="90"/>
+      <c r="I17" s="86"/>
     </row>
     <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="91"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="98" t="s">
+      <c r="B18" s="87"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="99"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="91"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
     </row>
     <row r="20" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
       <c r="F20" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="97">
+      <c r="G20" s="88">
         <f>SUM!C14</f>
         <v>0</v>
       </c>
-      <c r="H20" s="90"/>
-      <c r="I20" s="90"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
       <c r="F21" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="91"/>
-      <c r="H21" s="91"/>
-      <c r="I21" s="91"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
     </row>
     <row r="22" spans="1:9" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
@@ -2265,6 +2265,20 @@
     <row r="47" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="C8:I9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="G11:I12"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="B20:E21"/>
     <mergeCell ref="G20:I21"/>
     <mergeCell ref="A14:B14"/>
@@ -2273,20 +2287,6 @@
     <mergeCell ref="B17:E18"/>
     <mergeCell ref="H17:I18"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="C8:I9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="G11:I12"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:I6"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <phoneticPr fontId="40" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2353,19 +2353,19 @@
       <c r="K2" s="25"/>
     </row>
     <row r="3" spans="1:14" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
@@ -2422,32 +2422,32 @@
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="100" t="s">
+      <c r="D7" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="100" t="s">
+      <c r="E7" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="100" t="s">
+      <c r="F7" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="100" t="s">
+      <c r="G7" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="104" t="s">
+      <c r="H7" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="105"/>
-      <c r="J7" s="100" t="s">
+      <c r="I7" s="106"/>
+      <c r="J7" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="100" t="s">
+      <c r="K7" s="101" t="s">
         <v>9</v>
       </c>
       <c r="L7" s="2"/>
@@ -2455,20 +2455,20 @@
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="100"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
       <c r="L8" s="2"/>
       <c r="M8" s="8"/>
     </row>
@@ -2704,8 +2704,8 @@
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="C21" s="101"/>
-      <c r="D21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="103"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
@@ -2786,47 +2786,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="108" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
       <c r="Q1" s="72"/>
       <c r="R1" s="72"/>
       <c r="S1" s="72"/>
     </row>
     <row r="2" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
       <c r="Q2" s="73"/>
       <c r="R2" s="73"/>
       <c r="S2" s="73"/>
@@ -2837,18 +2837,18 @@
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
-      <c r="E3" s="108" t="str">
+      <c r="E3" s="143" t="str">
         <f>"报告期间：" &amp; N3 &amp; "至" &amp; N3</f>
         <v>报告期间：1900年1月0日至1900年1月0日</v>
       </c>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108" t="s">
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="108"/>
+      <c r="K3" s="143"/>
       <c r="L3" s="43"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70" t="str">
@@ -2862,17 +2862,17 @@
       <c r="S3" s="45"/>
     </row>
     <row r="4" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="145" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="145"/>
       <c r="D4" s="74"/>
       <c r="E4" s="74"/>
       <c r="F4" s="75"/>
       <c r="G4" s="76"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
       <c r="J4" s="71" t="s">
         <v>76</v>
       </c>
@@ -2887,68 +2887,68 @@
       <c r="P4" s="71"/>
     </row>
     <row r="5" spans="1:19" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="155" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="117" t="s">
+      <c r="C5" s="151" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="113" t="s">
+      <c r="D5" s="141" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="111" t="s">
+      <c r="E5" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="113" t="s">
+      <c r="F5" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="111" t="s">
+      <c r="G5" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="111" t="s">
+      <c r="H5" s="147" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="111" t="s">
+      <c r="I5" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="111" t="s">
+      <c r="J5" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="113" t="s">
+      <c r="K5" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="115" t="s">
+      <c r="L5" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="115" t="s">
+      <c r="M5" s="149" t="s">
         <v>42</v>
       </c>
-      <c r="N5" s="115"/>
+      <c r="N5" s="149"/>
       <c r="O5" s="59" t="s">
         <v>66</v>
       </c>
       <c r="P5" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="Q5" s="107"/>
-      <c r="R5" s="107"/>
+      <c r="Q5" s="144"/>
+      <c r="R5" s="144"/>
     </row>
     <row r="6" spans="1:19" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="122"/>
-      <c r="B6" s="120"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="116"/>
+      <c r="A6" s="156"/>
+      <c r="B6" s="154"/>
+      <c r="C6" s="152"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="148"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="142"/>
+      <c r="L6" s="150"/>
       <c r="M6" s="55" t="s">
         <v>43</v>
       </c>
@@ -2963,17 +2963,17 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
-      <c r="B7" s="120"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="114"/>
+      <c r="A7" s="156"/>
+      <c r="B7" s="154"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="142"/>
+      <c r="E7" s="148"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="148"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
+      <c r="K7" s="142"/>
       <c r="L7" s="56"/>
       <c r="M7" s="56"/>
       <c r="N7" s="56"/>
@@ -3385,31 +3385,31 @@
       <c r="A29" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="141">
+      <c r="B29" s="126">
         <f>B30+F30</f>
         <v>0</v>
       </c>
-      <c r="C29" s="142"/>
-      <c r="D29" s="143"/>
+      <c r="C29" s="127"/>
+      <c r="D29" s="128"/>
       <c r="E29" s="47" t="s">
         <v>30</v>
       </c>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
-      <c r="H29" s="127" t="s">
+      <c r="H29" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="128"/>
-      <c r="J29" s="129"/>
-      <c r="K29" s="147">
+      <c r="I29" s="113"/>
+      <c r="J29" s="114"/>
+      <c r="K29" s="132">
         <f>B31</f>
         <v>0</v>
       </c>
-      <c r="L29" s="148"/>
-      <c r="M29" s="148"/>
-      <c r="N29" s="148"/>
-      <c r="O29" s="148"/>
-      <c r="P29" s="149"/>
+      <c r="L29" s="133"/>
+      <c r="M29" s="133"/>
+      <c r="N29" s="133"/>
+      <c r="O29" s="133"/>
+      <c r="P29" s="134"/>
       <c r="Q29" s="48"/>
       <c r="R29" s="49"/>
     </row>
@@ -3417,29 +3417,29 @@
       <c r="A30" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="144">
+      <c r="B30" s="129">
         <f>L28</f>
         <v>0</v>
       </c>
-      <c r="C30" s="145"/>
-      <c r="D30" s="146"/>
+      <c r="C30" s="130"/>
+      <c r="D30" s="131"/>
       <c r="E30" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="144">
+      <c r="F30" s="129">
         <f>M28+N28</f>
         <v>0</v>
       </c>
-      <c r="G30" s="146"/>
-      <c r="H30" s="130"/>
-      <c r="I30" s="131"/>
-      <c r="J30" s="132"/>
-      <c r="K30" s="150"/>
-      <c r="L30" s="151"/>
-      <c r="M30" s="151"/>
-      <c r="N30" s="151"/>
-      <c r="O30" s="151"/>
-      <c r="P30" s="152"/>
+      <c r="G30" s="131"/>
+      <c r="H30" s="115"/>
+      <c r="I30" s="116"/>
+      <c r="J30" s="117"/>
+      <c r="K30" s="135"/>
+      <c r="L30" s="136"/>
+      <c r="M30" s="136"/>
+      <c r="N30" s="136"/>
+      <c r="O30" s="136"/>
+      <c r="P30" s="137"/>
       <c r="Q30" s="48"/>
       <c r="R30" s="49"/>
     </row>
@@ -3447,29 +3447,29 @@
       <c r="A31" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="136">
+      <c r="B31" s="121">
         <f>K28</f>
         <v>0</v>
       </c>
-      <c r="C31" s="137"/>
-      <c r="D31" s="138"/>
+      <c r="C31" s="122"/>
+      <c r="D31" s="123"/>
       <c r="E31" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="125">
+      <c r="F31" s="110">
         <f>D28</f>
         <v>0</v>
       </c>
-      <c r="G31" s="126"/>
-      <c r="H31" s="130"/>
-      <c r="I31" s="131"/>
-      <c r="J31" s="132"/>
-      <c r="K31" s="150"/>
-      <c r="L31" s="151"/>
-      <c r="M31" s="151"/>
-      <c r="N31" s="151"/>
-      <c r="O31" s="151"/>
-      <c r="P31" s="152"/>
+      <c r="G31" s="111"/>
+      <c r="H31" s="115"/>
+      <c r="I31" s="116"/>
+      <c r="J31" s="117"/>
+      <c r="K31" s="135"/>
+      <c r="L31" s="136"/>
+      <c r="M31" s="136"/>
+      <c r="N31" s="136"/>
+      <c r="O31" s="136"/>
+      <c r="P31" s="137"/>
       <c r="Q31" s="48"/>
       <c r="R31" s="49"/>
     </row>
@@ -3478,41 +3478,29 @@
         <v>38</v>
       </c>
       <c r="B32" s="68"/>
-      <c r="C32" s="139">
+      <c r="C32" s="124">
         <v>0</v>
       </c>
-      <c r="D32" s="140"/>
+      <c r="D32" s="125"/>
       <c r="E32" s="68" t="s">
         <v>39</v>
       </c>
       <c r="F32" s="68"/>
       <c r="G32" s="68"/>
-      <c r="H32" s="133"/>
-      <c r="I32" s="134"/>
-      <c r="J32" s="135"/>
-      <c r="K32" s="153"/>
-      <c r="L32" s="154"/>
-      <c r="M32" s="154"/>
-      <c r="N32" s="154"/>
-      <c r="O32" s="154"/>
-      <c r="P32" s="155"/>
+      <c r="H32" s="118"/>
+      <c r="I32" s="119"/>
+      <c r="J32" s="120"/>
+      <c r="K32" s="138"/>
+      <c r="L32" s="139"/>
+      <c r="M32" s="139"/>
+      <c r="N32" s="139"/>
+      <c r="O32" s="139"/>
+      <c r="P32" s="140"/>
       <c r="Q32" s="49"/>
       <c r="R32" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H29:J32"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="K29:P32"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E3:I3"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="A4:C4"/>
@@ -3529,6 +3517,18 @@
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="J5:J7"/>
     <mergeCell ref="E5:E7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H29:J32"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K29:P32"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E3:I3"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>